<commit_message>
template for steve 2025 data
</commit_message>
<xml_diff>
--- a/data-raw/bychick_2025_template.xlsx
+++ b/data-raw/bychick_2025_template.xlsx
@@ -1,76 +1,131 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/Git/kestrelbox/data-raw/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6EC0E03-0607-424E-810C-6E4944C07F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="1000" yWindow="780" windowWidth="21960" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="bychick_2025" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="bychick_2025" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t xml:space="preserve">box_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">weight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">band_date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fledge_date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">study_area</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXAMPLE1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024-05-23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024-06-04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central PA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXAMPLE2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024-06-13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024-06-24</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="33">
+  <si>
+    <t>box_id</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>band_date</t>
+  </si>
+  <si>
+    <t>fledge_date</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>study_area</t>
+  </si>
+  <si>
+    <t>EXAMPLE1</t>
+  </si>
+  <si>
+    <t>2024-05-23</t>
+  </si>
+  <si>
+    <t>2024-06-04</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Central PA</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>EXAMPLE10</t>
+  </si>
+  <si>
+    <t>2024-06-20</t>
+  </si>
+  <si>
+    <t>2024-06-21</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>EXAMPLE14</t>
+  </si>
+  <si>
+    <t>2024-06-25</t>
+  </si>
+  <si>
+    <t>2024-07-09</t>
+  </si>
+  <si>
+    <t>2024-07-11</t>
+  </si>
+  <si>
+    <t>2024-07-08</t>
+  </si>
+  <si>
+    <t>EXAMPLE24</t>
+  </si>
+  <si>
+    <t>2024-05-02</t>
+  </si>
+  <si>
+    <t>2024-05-19</t>
+  </si>
+  <si>
+    <t>2024-05-18</t>
+  </si>
+  <si>
+    <t>2024-05-20</t>
+  </si>
+  <si>
+    <t>EXAMPLE308</t>
+  </si>
+  <si>
+    <t>2024-07-16</t>
+  </si>
+  <si>
+    <t>2024-07-19</t>
+  </si>
+  <si>
+    <t>Lancaster</t>
+  </si>
+  <si>
+    <t>2024-07-20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -79,15 +134,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <b/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -129,6 +186,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -410,14 +476,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,17 +511,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C2" s="2" t="n">
+      <c r="B2" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C2" s="2">
         <v>18</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="2">
         <v>145</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -469,17 +537,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C3" s="2" t="n">
+      <c r="B3" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C3" s="2">
         <v>18</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="2">
         <v>148</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -495,17 +563,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C4" s="2" t="n">
+      <c r="B4" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C4" s="2">
         <v>18</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="2">
         <v>139</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -521,25 +589,25 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="2" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>19</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>110</v>
+      <c r="B5" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C5" s="2">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2">
+        <v>109</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="G5" s="2" t="s">
         <v>13</v>
       </c>
@@ -547,24 +615,24 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="2" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C6" s="2" t="n">
-        <v>19</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>126</v>
+      <c r="B6" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C6" s="2">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2">
+        <v>110</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>11</v>
@@ -573,128 +641,500 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7"/>
-      <c r="B7" t="n">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C7" s="2">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2">
+        <v>93</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C8" s="2">
+        <v>13</v>
+      </c>
+      <c r="D8" s="2">
+        <v>109</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C9" s="2">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2">
+        <v>118</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C10" s="2">
+        <v>15</v>
+      </c>
+      <c r="D10" s="2">
+        <v>104</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C11" s="2">
+        <v>13</v>
+      </c>
+      <c r="D11" s="2">
+        <v>92</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C12" s="2">
+        <v>16</v>
+      </c>
+      <c r="D12" s="2">
+        <v>121</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C13" s="2">
+        <v>15</v>
+      </c>
+      <c r="D13" s="2">
+        <v>118</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C14" s="2">
+        <v>13</v>
+      </c>
+      <c r="D14" s="2">
+        <v>107</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C15" s="2">
+        <v>14</v>
+      </c>
+      <c r="D15" s="2">
+        <v>117</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C16" s="2">
+        <v>13</v>
+      </c>
+      <c r="D16" s="2">
+        <v>109</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C17" s="2">
+        <v>12</v>
+      </c>
+      <c r="D17" s="2">
+        <v>101</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C18" s="2">
+        <v>12</v>
+      </c>
+      <c r="D18" s="2">
+        <v>104</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C19" s="2">
+        <v>27</v>
+      </c>
+      <c r="D19" s="2">
+        <v>108</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C20" s="2">
+        <v>26</v>
+      </c>
+      <c r="D20" s="2">
+        <v>100</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C21" s="2">
+        <v>27</v>
+      </c>
+      <c r="D21" s="2">
+        <v>100</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C22" s="2">
+        <v>26</v>
+      </c>
+      <c r="D22" s="2">
+        <v>104</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C23" s="2">
+        <v>27</v>
+      </c>
+      <c r="D23" s="2">
+        <v>106</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B24">
         <v>2025</v>
       </c>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7"/>
-    </row>
-    <row r="8">
-      <c r="A8"/>
-      <c r="B8" t="n">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B25">
         <v>2025</v>
       </c>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
-      <c r="G8"/>
-      <c r="H8"/>
-    </row>
-    <row r="9">
-      <c r="A9"/>
-      <c r="B9" t="n">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B26">
         <v>2025</v>
       </c>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9"/>
-      <c r="G9"/>
-      <c r="H9"/>
-    </row>
-    <row r="10">
-      <c r="A10"/>
-      <c r="B10" t="n">
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B27">
         <v>2025</v>
       </c>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
-      <c r="H10"/>
-    </row>
-    <row r="11">
-      <c r="A11"/>
-      <c r="B11" t="n">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B28">
         <v>2025</v>
       </c>
-      <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11"/>
-      <c r="H11"/>
-    </row>
-    <row r="12">
-      <c r="A12"/>
-      <c r="B12" t="n">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B29">
         <v>2025</v>
       </c>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
-      <c r="G12"/>
-      <c r="H12"/>
-    </row>
-    <row r="13">
-      <c r="A13"/>
-      <c r="B13" t="n">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B30">
         <v>2025</v>
       </c>
-      <c r="C13"/>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
-      <c r="G13"/>
-      <c r="H13"/>
-    </row>
-    <row r="14">
-      <c r="A14"/>
-      <c r="B14" t="n">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B31">
         <v>2025</v>
       </c>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14"/>
-      <c r="G14"/>
-      <c r="H14"/>
-    </row>
-    <row r="15">
-      <c r="A15"/>
-      <c r="B15" t="n">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B32">
         <v>2025</v>
       </c>
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15"/>
-      <c r="F15"/>
-      <c r="G15"/>
-      <c r="H15"/>
-    </row>
-    <row r="16">
-      <c r="A16"/>
-      <c r="B16" t="n">
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33">
         <v>2025</v>
       </c>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16"/>
-      <c r="G16"/>
-      <c r="H16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>